<commit_message>
report + comments on task
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -54,7 +54,8 @@
 3- For search on disponible flights, client needs to consult Vol first! So client needs to have access to class Vol. (maybe using an application class with is like a connector between client and another composents ---- see Demo4)
 4- add access methods on associations.(see Demo4)
 5- I need your explanation about this diagram! for instance; I don't understand ControlReservation!
-6- We need to add methods for every operation which are explicitly mentioned in the wording. such as rechercheVol. In fact diag de classe should be matched with diags de sequences</t>
+6- We need to add methods for every operation which are explicitly mentioned in the wording. such as rechercheVol. In fact diag de classe should be matched with diags de sequences
+7- Don't forget the rule of attributes that I explained to you last saturday</t>
         </r>
       </text>
     </comment>
@@ -716,7 +717,7 @@
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1216,13 +1217,13 @@
         <v>6</v>
       </c>
       <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">

</xml_diff>

<commit_message>
Updated and ompleted system sequence diagrams in report
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matiar\git\ift3911-dm1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{9C8A502C-B0B4-411C-9F1D-013673064827}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,12 +19,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Matiar</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{22411DA5-907E-4D82-877F-C1BA44C7A924}">
+    <comment ref="C3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{2EEECA22-0C35-4D2A-8FCE-8663FA2445AA}">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -80,11 +75,11 @@
           </rPr>
           <t xml:space="preserve">
 I believe you had these diags but I couldn't find them
-</t>
+Lyia: Included in the report and added jpg files.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{980B8B70-992F-4040-B9DE-7F6559BFCDBD}">
+    <comment ref="C16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,11 +99,12 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-missing</t>
+missing
+Lygia: I think this is included in "modifier vol", or "créer vol"</t>
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{B64D289D-0DC1-467A-A01F-319980C8CCED}">
+    <comment ref="C28" authorId="0">
       <text>
         <r>
           <rPr>
@@ -133,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{306A2507-8369-4CC2-9EAB-D14D8AE8E5C4}">
+    <comment ref="C29" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +293,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -706,18 +702,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B64CB90-6068-4832-A517-F4347FDDCFF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated class diagram implementation and sequence diagrams
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -124,8 +124,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">It should be related to section and finaly seat to check if there is any seat left of the desired class selected by the client. (look at mine!)
-</t>
+          <t>It should be related to section and finaly seat to check if there is any seat left of the desired class selected by the client. (look at mine!)
+Lygia: Done</t>
         </r>
       </text>
     </comment>
@@ -150,7 +150,8 @@
           </rPr>
           <t xml:space="preserve">
 There is no message back to the client
-We need also save the current time when the reservation is done for taking care of the 24h condition! Maybe a self calling function on reservation!</t>
+We need also save the current time when the reservation is done for taking care of the 24h condition! Maybe a self calling function on reservation!
+Lygia: Done</t>
         </r>
       </text>
     </comment>
@@ -712,8 +713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,7 +1112,7 @@
       <c r="B30" s="1">
         <v>4.3</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -1137,7 +1138,7 @@
       <c r="B32" s="1">
         <v>4.5</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D32" s="1" t="s">

</xml_diff>

<commit_message>
update contrat+diag de class+ocl
</commit_message>
<xml_diff>
--- a/taches.xlsx
+++ b/taches.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matiar\git\ift3911-dm1\ift3911-dm1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9048" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Matiar</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,16 +50,14 @@
           </rPr>
           <t xml:space="preserve">
 1- Admin is not connected to any class
-2- I didn't understand what is exactly catalouge!
-3- For search on disponible flights, client needs to consult Vol first! So client needs to have access to class Vol. (maybe using an application class with is like a connector between client and another composents ---- see Demo4)
-4- add access methods on associations.(see Demo4)
-5- I need your explanation about this diagram! for instance; I don't understand ControlReservation!
-6- We need to add methods for every operation which are explicitly mentioned in the wording. such as rechercheVol. In fact diag de classe should be matched with diags de sequences
-7- Don't forget the rule of attributes that I explained to you last saturday</t>
+2- For search on disponible flights, client needs to consult Vol first! So client needs to have access to class Vol. (maybe using an application class with is like a connector between client and another composents ---- see Demo4)
+3- add access methods on associations.(see Demo4)
+4- We need to add methods for every operation which are explicitly mentioned in the wording. such as rechercheVol. In fact diag de classe should be matched with diags de sequences
+5- Don't forget the rule of attributes that I explained to you last saturday</t>
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0">
+    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +82,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C16" authorId="0">
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -104,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C28" authorId="0">
+    <comment ref="C28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -129,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C29" authorId="0">
+    <comment ref="C29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -294,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -703,18 +706,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>